<commit_message>
Added class examples for dataframe merging, concatenating, and some erroneous items.  Added in-class examples for students to try.
</commit_message>
<xml_diff>
--- a/Session 7 - Python/Instructional Material/Class Examples/Pandas/food_data.xlsx
+++ b/Session 7 - Python/Instructional Material/Class Examples/Pandas/food_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doug\Repositories\PracticalProgramming\Session 7 - Python\Instructional Material\Class Examples\Pandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{723C8DC4-ACEE-4895-A78B-12D98F0767FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C11C9AC-3EDA-4F34-A14B-C7AAA60D39D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="833" windowWidth="11175" windowHeight="9232"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="food_data" sheetId="1" r:id="rId1"/>
+    <sheet name="stock_data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Food</t>
   </si>
@@ -53,12 +54,15 @@
   </si>
   <si>
     <t>oz</t>
+  </si>
+  <si>
+    <t>Amount Available (lb)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -892,10 +896,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -968,4 +974,67 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7AE4143-B0F3-4035-896F-0956CD0B51CA}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>